<commit_message>
Cleaning up the incompatible types mess
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/smallwares/PickList.xlsx
+++ b/WorkBot/main/backend/smallwares/PickList.xlsx
@@ -529,7 +529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H1303"/>
+  <dimension ref="A1:H1335"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A669" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F693" sqref="F693"/>
@@ -34286,10 +34286,972 @@
           <t xml:space="preserve"> 1</t>
         </is>
       </c>
-      <c r="F1303" t="inlineStr"/>
-      <c r="G1303" t="inlineStr"/>
       <c r="H1303" t="n">
         <v>99</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>110TWN09180</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>Twinings Lemon &amp; Ginger Herbal Tea Bags - 25/Box</t>
+        </is>
+      </c>
+      <c r="E1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="H1304" t="n">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>110TWN09181</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>Twinings English Breakfast Tea Bags - 25/Box</t>
+        </is>
+      </c>
+      <c r="E1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 24</t>
+        </is>
+      </c>
+      <c r="H1305" t="n">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>110TWN09183</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>Twinings Earl Grey Tea Bags - 25/Box</t>
+        </is>
+      </c>
+      <c r="E1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="H1306" t="n">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>40862028</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>Ghirardelli 30 lb. Sweet Ground Chocolate &amp; Cocoa Powder</t>
+        </is>
+      </c>
+      <c r="E1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5</t>
+        </is>
+      </c>
+      <c r="H1307" t="n">
+        <v>123.47</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>8808604CS</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>Torani Puremade White Chocolate Flavoring Sauce 64 fl. oz. - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H1308" t="n">
+        <v>72.98999999999999</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>8808605CS</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>Torani Puremade Dark Chocolate Flavoring Sauce 64 fl. oz. - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1309" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="H1309" t="n">
+        <v>67.98999999999999</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>110TWN05328</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>Twinings Irish Breakfast Tea Bags - 20/Box</t>
+        </is>
+      </c>
+      <c r="E1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="H1310" t="n">
+        <v>4.39</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>711SPRNKLEPK</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>Adourne Pink Sprinkles 10 lb.</t>
+        </is>
+      </c>
+      <c r="E1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1311" t="n">
+        <v>25.62</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>107750625</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>110TWN09183</t>
+        </is>
+      </c>
+      <c r="D1312" t="inlineStr">
+        <is>
+          <t>Twinings Earl Grey Tea Bags - 25/Box</t>
+        </is>
+      </c>
+      <c r="E1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="H1312" t="n">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 17, 2025</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>107750760</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>323CIRCL2018</t>
+        </is>
+      </c>
+      <c r="D1313" t="inlineStr">
+        <is>
+          <t>Lavex 2" Fluorescent Green Matte Paper Permanent Round Inventory Label - 500/Roll</t>
+        </is>
+      </c>
+      <c r="E1313" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 12</t>
+        </is>
+      </c>
+      <c r="H1313" t="n">
+        <v>6.489999999999999</v>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>150BB6218N</t>
+        </is>
+      </c>
+      <c r="D1314" t="inlineStr">
+        <is>
+          <t>Durable Packaging BB6218N 18" x 6" x 3 1/4" Kraft Paper Windowed Bread Bag - 1000/Case</t>
+        </is>
+      </c>
+      <c r="E1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1314" t="n">
+        <v>104.99</v>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>43306LPIE300</t>
+        </is>
+      </c>
+      <c r="D1315" t="inlineStr">
+        <is>
+          <t>Choice 6" Clear Hinged Pie Container with Low Dome Lid - 300/Case</t>
+        </is>
+      </c>
+      <c r="E1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="H1315" t="n">
+        <v>49.99</v>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>150300865</t>
+        </is>
+      </c>
+      <c r="D1316" t="inlineStr">
+        <is>
+          <t>Bagcraft Packaging 300865 EcoCraft 6" x 3 1/2" x 13 1/2" Dubl Panel® Artisan Bread Bag - 500/Case</t>
+        </is>
+      </c>
+      <c r="E1316" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1316" t="n">
+        <v>79.98999999999999</v>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>500CTOUT160</t>
+        </is>
+      </c>
+      <c r="D1317" t="inlineStr">
+        <is>
+          <t>Choice 160 oz. Beverage Take-Out Container - 20/Case</t>
+        </is>
+      </c>
+      <c r="E1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H1317" t="n">
+        <v>94.99000000000001</v>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>433QLINERBL</t>
+        </is>
+      </c>
+      <c r="D1318" t="inlineStr">
+        <is>
+          <t>Baker's Lane 16" x 24" Full Size Quilon® Coated Parchment Paper Bun / Sheet Pan Liner Sheet - 1000/Case</t>
+        </is>
+      </c>
+      <c r="E1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="H1318" t="n">
+        <v>45.99</v>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 18, 2025</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>107786615</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>433SLINERBL</t>
+        </is>
+      </c>
+      <c r="D1319" t="inlineStr">
+        <is>
+          <t>Baker's Lane 16" x 24" Full Size Silicone Coated Parchment Paper Bun / Sheet Pan Liner Sheet - 1000/Case</t>
+        </is>
+      </c>
+      <c r="E1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="H1319" t="n">
+        <v>76.98999999999999</v>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 19, 2025</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>107836987</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>8808606CS</t>
+        </is>
+      </c>
+      <c r="D1320" t="inlineStr">
+        <is>
+          <t>Torani Puremade Caramel Flavoring Sauce 64 fl. oz. - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="H1320" t="n">
+        <v>72.98999999999999</v>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>844CBBLKNBR35</t>
+        </is>
+      </c>
+      <c r="D1321" t="inlineStr">
+        <is>
+          <t>Lavex 3' x 5' Heavy-Duty Black Grease-Resistant Anti-Fatigue Closed-Cell Nitrile Rubber Floor Mat - 3/4" Thick</t>
+        </is>
+      </c>
+      <c r="E1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1321" t="n">
+        <v>92.98999999999999</v>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>697STW60</t>
+        </is>
+      </c>
+      <c r="D1322" t="inlineStr">
+        <is>
+          <t>Lavex 60" Wooden Mop Handle with Stirrup-Style End</t>
+        </is>
+      </c>
+      <c r="E1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H1322" t="n">
+        <v>7.989999999999999</v>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>544SYPFR145K</t>
+        </is>
+      </c>
+      <c r="D1323" t="inlineStr">
+        <is>
+          <t>Monin Premium Toasted Marshmallow Flavoring Syrup 1 Liter - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1323" t="n">
+        <v>37.99</v>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>544SYPFR023K</t>
+        </is>
+      </c>
+      <c r="D1324" t="inlineStr">
+        <is>
+          <t>Monin Premium Hazelnut Flavoring Syrup 1 Liter - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1324" t="n">
+        <v>38.49</v>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>544SYPAR012KT</t>
+        </is>
+      </c>
+      <c r="D1325" t="inlineStr">
+        <is>
+          <t>Monin Premium Cinnamon Flavoring Syrup 750 mL - 12/Case</t>
+        </is>
+      </c>
+      <c r="E1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H1325" t="n">
+        <v>86.98999999999999</v>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>544SYPAR258KT</t>
+        </is>
+      </c>
+      <c r="D1326" t="inlineStr">
+        <is>
+          <t>Monin Premium Butter Pecan Flavoring Syrup 750 mL - 12/Case</t>
+        </is>
+      </c>
+      <c r="E1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1326" t="n">
+        <v>86.98999999999999</v>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>110TWN08465KT</t>
+        </is>
+      </c>
+      <c r="D1327" t="inlineStr">
+        <is>
+          <t>Twinings Pomegranate &amp; Raspberry Herbal Tea Bags - 120/Case</t>
+        </is>
+      </c>
+      <c r="E1327" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1327" t="n">
+        <v>21.99</v>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>182RRF8</t>
+        </is>
+      </c>
+      <c r="D1328" t="inlineStr">
+        <is>
+          <t>Choice 6 1/2" x 7 3/4" Plastic Food Bag on a Roll - 2000/Case</t>
+        </is>
+      </c>
+      <c r="E1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6</t>
+        </is>
+      </c>
+      <c r="H1328" t="n">
+        <v>19.29</v>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>110TWN05322KT</t>
+        </is>
+      </c>
+      <c r="D1329" t="inlineStr">
+        <is>
+          <t>Twinings Darjeeling Tea Bags - 120/Case</t>
+        </is>
+      </c>
+      <c r="E1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2</t>
+        </is>
+      </c>
+      <c r="H1329" t="n">
+        <v>21.99</v>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 23, 2025</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>107965562</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>8808607CS</t>
+        </is>
+      </c>
+      <c r="D1330" t="inlineStr">
+        <is>
+          <t>Torani Puremade Pumpkin Pie Flavoring Sauce 64 fl. oz. - 4/Case</t>
+        </is>
+      </c>
+      <c r="E1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="H1330" t="n">
+        <v>72.98999999999999</v>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 26, 2025</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>108078832</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>612H18A</t>
+        </is>
+      </c>
+      <c r="D1331" t="inlineStr">
+        <is>
+          <t>Durable Packaging High Dome Plastic Cover for 1/4 Sheet Cake Pan - 100/Case</t>
+        </is>
+      </c>
+      <c r="E1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="H1331" t="n">
+        <v>50.99</v>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 26, 2025</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>108078832</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>612604245</t>
+        </is>
+      </c>
+      <c r="D1332" t="inlineStr">
+        <is>
+          <t>Durable Packaging 1/4 Sheet Foil Cake Pan - 100/Case</t>
+        </is>
+      </c>
+      <c r="E1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8</t>
+        </is>
+      </c>
+      <c r="H1332" t="n">
+        <v>48.99</v>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 26, 2025</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>108078832</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>111QUINTRORG</t>
+        </is>
+      </c>
+      <c r="D1333" t="inlineStr">
+        <is>
+          <t>Organic Tri-Color Quinoa - 25 lb.</t>
+        </is>
+      </c>
+      <c r="E1333" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="H1333" t="n">
+        <v>62.11000000000001</v>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 26, 2025</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>108082685</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>697JWMH60GN</t>
+        </is>
+      </c>
+      <c r="D1334" t="inlineStr">
+        <is>
+          <t>Lavex 60" Green Jaw Style Metal Mop Handle</t>
+        </is>
+      </c>
+      <c r="E1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 3</t>
+        </is>
+      </c>
+      <c r="F1334" t="inlineStr"/>
+      <c r="G1334" t="inlineStr"/>
+      <c r="H1334" t="n">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> February 26, 2025</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>108082685</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>697QMH60GN</t>
+        </is>
+      </c>
+      <c r="D1335" t="inlineStr">
+        <is>
+          <t>Lavex 60" Green Quick Release Metal Mop Handle</t>
+        </is>
+      </c>
+      <c r="E1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="F1335" t="inlineStr"/>
+      <c r="G1335" t="inlineStr"/>
+      <c r="H1335" t="n">
+        <v>7.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>